<commit_message>
Added sensor port mapping, trigger decoding from sequence file
</commit_message>
<xml_diff>
--- a/Test Sequences/Test Sequence 1.xlsx
+++ b/Test Sequences/Test Sequence 1.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="__SETUP__" sheetId="4" r:id="rId2"/>
+    <sheet name="Abort" sheetId="5" r:id="rId2"/>
+    <sheet name="__SETUP__" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="TestSeqActions" localSheetId="1">Abort!$D$4:$D$1048576</definedName>
     <definedName name="TestSeqActions">Main!$D$4:$D$1048576</definedName>
+    <definedName name="TestSeqTimes" localSheetId="1">Abort!$B$4:$B$1048576</definedName>
     <definedName name="TestSeqTimes">Main!$B$4:$B$1048576</definedName>
+    <definedName name="TestSeqValves" localSheetId="1">Abort!$C$4:$C$1048576</definedName>
     <definedName name="TestSeqValves" localSheetId="0">Main!$C$4:$C$1048576</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -193,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -202,6 +206,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -215,7 +222,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -514,8 +535,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,20 +554,20 @@
   <sheetData>
     <row r="1" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="2:11" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -595,7 +616,7 @@
         <v>2000</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -624,7 +645,7 @@
         <v>50000</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -686,10 +707,10 @@
     <mergeCell ref="F2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="CLOSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="CLOSE">
       <formula>NOT(ISERROR(SEARCH("CLOSE",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -735,6 +756,229 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="2:11" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>500</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:K2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:E1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="CLOSE">
+      <formula>NOT(ISERROR(SEARCH("CLOSE",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="whole" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1048576">
+      <formula1>9889898988</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1048576">
+      <formula1>9999889</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576">
+      <formula1>9999921</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>__SETUP__!$C$4:$C$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>H4:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>__SETUP__!$D$4:$D$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>__SETUP__!$B$4:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:D11"/>
   <sheetViews>
@@ -746,11 +990,11 @@
   <sheetData>
     <row r="1" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">

</xml_diff>